<commit_message>
Adjust backlog to meet the change with user stories.
</commit_message>
<xml_diff>
--- a/Docs/product backlog.xlsx
+++ b/Docs/product backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13920"/>
+    <workbookView windowWidth="23040" windowHeight="9420"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Story ID</t>
   </si>
@@ -136,29 +136,30 @@
     <t>2.3.2.1</t>
   </si>
   <si>
-    <t>Story 2.3.2.1</t>
+    <t>Story 2.3.3.1</t>
   </si>
   <si>
     <t>As a airport staff
-  I want a tag that needs to be attached to the carry-on baggage
-  So that I can record and check the weight and contents of the luggage during the security check to ensure the safety of the flight</t>
-  </si>
-  <si>
-    <t>The tag needs to have the information including the flight number, destination, departure, and the ID of the baggage tag</t>
-  </si>
-  <si>
-    <t>2.3.2.2</t>
-  </si>
-  <si>
-    <t>Story 2.3.2.2</t>
-  </si>
-  <si>
-    <t>As a passenger with a plain suitcase  
-I want a tag that needs to be attached to the carry-on baggage
-  So that  I can find my own luggage by matching the tag on my boarding pass to the tag on my suitcase</t>
-  </si>
-  <si>
-    <t>The tag needs to have the information including the ID of the baggage tag</t>
+I want a ticket that needs to be attached to the check-in baggage
+So that I can record and check the weight and contents of the luggage during the security check to ensure the safety of the flight</t>
+  </si>
+  <si>
+    <t>The ticket needs to have the information including the flight number, destination, departure, and the ID of the baggage tag</t>
+  </si>
+  <si>
+    <t>2.3.3.2</t>
+  </si>
+  <si>
+    <t>Story 2.3.3.2</t>
+  </si>
+  <si>
+    <t>As a Businessman
+I want a ticket with the number of the assigned bag drop counter where the passenger needs to go to drop his/her check-in baggage
+So that I can faster access to bag drop counter information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tickets are printed with adhesive material on the back, giving passengers the option to attach their tickets to their boarding passes without losing them
+</t>
   </si>
   <si>
     <t>2.1.2</t>
@@ -191,19 +192,18 @@
 ·Verify that the additional price can be displayed.</t>
   </si>
   <si>
-    <t>2.3.3</t>
-  </si>
-  <si>
-    <t>Story 2.3.3</t>
-  </si>
-  <si>
-    <t>As a Businessman
-  I want a ticket with the number of the assigned bag drop counter where the passenger needs to go to drop his/her check-in baggage
-  So that  I can faster access to bag drop counter information</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tickets are printed with adhesive material on the back, giving passengers the option to attach their tickets to their boarding passes without losing them
-</t>
+    <t>2.3.2</t>
+  </si>
+  <si>
+    <t>Story 2.3.2</t>
+  </si>
+  <si>
+    <t>As a passenger with a plain suitcase  
+I want a tag that needs to be attached to the carry-on baggage
+So that I can find my own luggage by checking the tag on my suitcase, and the baggage won’t be taken in error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The tag needs to have the information including the surname of  passenger and the number of the baggage </t>
   </si>
   <si>
     <t>Story 2.4</t>
@@ -241,11 +241,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,14 +268,42 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -284,30 +312,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -330,63 +352,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -398,15 +367,39 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -427,61 +420,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -493,115 +588,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -639,13 +632,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -674,41 +686,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -727,222 +709,230 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="47" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="47" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="36" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="36" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
-    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
-    <cellStyle name="输入" xfId="4" builtinId="20"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
-    <cellStyle name="货币" xfId="7" builtinId="4"/>
-    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
-    <cellStyle name="百分比" xfId="9" builtinId="5"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
-    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
-    <cellStyle name="计算" xfId="15" builtinId="22"/>
-    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
-    <cellStyle name="适中" xfId="17" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
-    <cellStyle name="好" xfId="19" builtinId="26"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="差" xfId="22" builtinId="27"/>
-    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
     <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
-    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
-    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
-    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
-    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
-    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
-    <cellStyle name="标题" xfId="33" builtinId="15"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
-    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="注释" xfId="37" builtinId="10"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
-    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
-    <cellStyle name="超链接" xfId="41" builtinId="8"/>
-    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
-    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
     <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
     <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
-    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -1238,24 +1228,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
-      <selection activeCell="D1" sqref="D$1:D$1048576"/>
+    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="10.9134615384615" customWidth="1"/>
-    <col min="2" max="2" width="16.7115384615385" customWidth="1"/>
+    <col min="1" max="1" width="10.9166666666667" customWidth="1"/>
+    <col min="2" max="2" width="16.712962962963" customWidth="1"/>
     <col min="3" max="3" width="36" customWidth="1"/>
-    <col min="5" max="5" width="28.4230769230769" customWidth="1"/>
-    <col min="6" max="6" width="37.7019230769231" customWidth="1"/>
-    <col min="7" max="7" width="17.1442307692308" customWidth="1"/>
-    <col min="8" max="8" width="24.8557692307692" customWidth="1"/>
-    <col min="9" max="9" width="26.2884615384615" customWidth="1"/>
+    <col min="5" max="5" width="28.4259259259259" customWidth="1"/>
+    <col min="6" max="6" width="37.7037037037037" customWidth="1"/>
+    <col min="7" max="7" width="17.1481481481481" customWidth="1"/>
+    <col min="8" max="8" width="24.8518518518519" customWidth="1"/>
+    <col min="9" max="9" width="26.287037037037" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1303,18 +1293,18 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" ht="118" spans="1:6">
+    <row r="3" ht="115.2" spans="1:6">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D3">
@@ -1323,18 +1313,18 @@
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" ht="118" spans="1:6">
+    <row r="4" ht="115.2" spans="1:6">
       <c r="A4" t="s">
         <v>17</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D4">
@@ -1343,18 +1333,18 @@
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" ht="68" spans="1:6">
+    <row r="5" ht="57.6" spans="1:6">
       <c r="A5" t="s">
         <v>21</v>
       </c>
       <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D5">
@@ -1363,18 +1353,18 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" ht="101" spans="1:6">
+    <row r="6" ht="100.8" spans="1:6">
       <c r="A6" t="s">
         <v>25</v>
       </c>
       <c r="B6" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D6">
@@ -1383,18 +1373,18 @@
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" ht="84" spans="1:6">
+    <row r="7" ht="86.4" spans="1:6">
       <c r="A7" t="s">
         <v>29</v>
       </c>
       <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D7">
@@ -1403,18 +1393,18 @@
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" ht="118" spans="1:6">
+    <row r="8" ht="100.8" spans="1:6">
       <c r="A8" t="s">
         <v>33</v>
       </c>
       <c r="B8" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D8">
@@ -1423,18 +1413,18 @@
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="9" ht="101" spans="1:6">
+    <row r="9" ht="100.8" spans="1:6">
       <c r="A9" t="s">
         <v>37</v>
       </c>
       <c r="B9" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D9">
@@ -1443,18 +1433,18 @@
       <c r="E9">
         <v>1</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" ht="88" spans="1:6">
+    <row r="10" ht="93.6" spans="1:6">
       <c r="A10" t="s">
         <v>41</v>
       </c>
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D10">
@@ -1463,18 +1453,18 @@
       <c r="E10">
         <v>1</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" ht="101" spans="1:6">
+    <row r="11" ht="86.4" spans="1:6">
       <c r="A11" t="s">
         <v>45</v>
       </c>
       <c r="B11" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>47</v>
       </c>
       <c r="D11">
@@ -1483,18 +1473,18 @@
       <c r="E11">
         <v>1</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" ht="118" spans="1:6">
+    <row r="12" ht="115.2" spans="1:6">
       <c r="A12" t="s">
         <v>49</v>
       </c>
       <c r="B12" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>51</v>
       </c>
       <c r="D12">
@@ -1503,18 +1493,18 @@
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" ht="101" spans="1:6">
-      <c r="A13" s="5">
+    <row r="13" ht="100.8" spans="1:6">
+      <c r="A13" s="6">
         <v>2.4</v>
       </c>
       <c r="B13" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D13">
@@ -1523,18 +1513,18 @@
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" ht="101" spans="1:6">
+    <row r="14" ht="100.8" spans="1:6">
       <c r="A14" t="s">
         <v>56</v>
       </c>
       <c r="B14" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>58</v>
       </c>
       <c r="D14">
@@ -1543,7 +1533,7 @@
       <c r="E14">
         <v>1</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="3" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update product backlog file
</commit_message>
<xml_diff>
--- a/Docs/product backlog.xlsx
+++ b/Docs/product backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EBU6304-2021-Software-Engineering-Group-111\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jerry\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5F593F-64AA-4D64-8315-63CE16EA575A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10F20E6-19BB-4153-B844-1D2990CFED60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -653,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -795,8 +795,12 @@
       <c r="F5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="H5" s="7">
+        <v>44649</v>
+      </c>
+      <c r="I5" s="7">
+        <v>44649</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="100.8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">

</xml_diff>

<commit_message>
Added Story 2.7.docx, and optimized the backlog
</commit_message>
<xml_diff>
--- a/Docs/product backlog.xlsx
+++ b/Docs/product backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13920"/>
+    <workbookView windowWidth="23040" windowHeight="9420"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="80">
   <si>
     <t>Story ID</t>
   </si>
@@ -300,6 +300,18 @@
   </si>
   <si>
     <t>- Verify that the clock wouldn't stop</t>
+  </si>
+  <si>
+    <t>Add QR code</t>
+  </si>
+  <si>
+    <t>As a passenger
+I want a QR code at the final page
+So that I can get more information about my trip on the website of the airline</t>
+  </si>
+  <si>
+    <t>-Verify that the QR code is generated by the name of user's airline automatically
+-Verify that the information in the QR code is correct</t>
   </si>
 </sst>
 </file>
@@ -308,9 +320,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -334,7 +346,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -344,6 +370,21 @@
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -355,8 +396,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -364,13 +421,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -384,6 +434,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -392,8 +458,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -409,38 +476,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -452,37 +495,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -499,13 +511,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -517,19 +655,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -541,139 +679,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -702,11 +714,28 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -735,47 +764,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -799,158 +787,185 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="36" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -959,29 +974,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -989,54 +1013,54 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
-    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
-    <cellStyle name="输入" xfId="4" builtinId="20"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
-    <cellStyle name="货币" xfId="7" builtinId="4"/>
-    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
-    <cellStyle name="百分比" xfId="9" builtinId="5"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
-    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
-    <cellStyle name="计算" xfId="15" builtinId="22"/>
-    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
-    <cellStyle name="适中" xfId="17" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
-    <cellStyle name="好" xfId="19" builtinId="26"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="差" xfId="22" builtinId="27"/>
-    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
     <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
-    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
-    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
-    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
-    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
-    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
-    <cellStyle name="标题" xfId="33" builtinId="15"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
-    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="注释" xfId="37" builtinId="10"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
-    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
-    <cellStyle name="超链接" xfId="41" builtinId="8"/>
-    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
-    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
     <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
     <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
-    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -1332,25 +1356,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" topLeftCell="C18" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="10.8846153846154" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.3365384615385" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.8888888888889" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.3333333333333" style="2" customWidth="1"/>
     <col min="3" max="3" width="36" style="2" customWidth="1"/>
     <col min="4" max="4" width="9" style="2"/>
-    <col min="5" max="5" width="21.8846153846154" style="2" customWidth="1"/>
-    <col min="6" max="6" width="37.6634615384615" style="3" customWidth="1"/>
-    <col min="7" max="7" width="6.10576923076923" style="2" customWidth="1"/>
-    <col min="8" max="8" width="24.8846153846154" style="2" customWidth="1"/>
-    <col min="9" max="9" width="26.3365384615385" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.8888888888889" style="2" customWidth="1"/>
+    <col min="6" max="6" width="37.6666666666667" style="3" customWidth="1"/>
+    <col min="7" max="7" width="6.10185185185185" style="2" customWidth="1"/>
+    <col min="8" max="8" width="24.8888888888889" style="2" customWidth="1"/>
+    <col min="9" max="9" width="26.3333333333333" style="2" customWidth="1"/>
     <col min="10" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
@@ -1370,7 +1394,7 @@
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
@@ -1383,517 +1407,544 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" ht="66" spans="1:9">
-      <c r="A2" s="5" t="s">
+    <row r="2" ht="69" spans="1:9">
+      <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="6">
         <v>1</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="6">
         <v>1</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="12">
+      <c r="G2" s="6"/>
+      <c r="H2" s="9">
         <v>44638</v>
       </c>
-      <c r="I2" s="12">
+      <c r="I2" s="9">
         <v>44644</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" ht="66" spans="1:9">
-      <c r="A3" s="7" t="s">
+    <row r="3" s="1" customFormat="1" ht="69" spans="1:9">
+      <c r="A3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="10">
         <v>1</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="10">
         <v>1</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="14">
+      <c r="G3" s="10"/>
+      <c r="H3" s="13">
         <v>44639</v>
       </c>
-      <c r="I3" s="14">
+      <c r="I3" s="13">
         <v>44641</v>
       </c>
     </row>
-    <row r="4" ht="93" spans="1:9">
-      <c r="A4" s="5" t="s">
+    <row r="4" ht="96.6" spans="1:9">
+      <c r="A4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="6">
         <v>1</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="12">
+      <c r="G4" s="6"/>
+      <c r="H4" s="9">
         <v>44639</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="9">
         <v>44643</v>
       </c>
     </row>
-    <row r="5" ht="53" spans="1:9">
-      <c r="A5" s="5" t="s">
+    <row r="5" ht="41.4" spans="1:9">
+      <c r="A5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="6">
         <v>1</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="6">
         <v>1</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="12">
+      <c r="G5" s="6"/>
+      <c r="H5" s="9">
         <v>44649</v>
       </c>
-      <c r="I5" s="12">
+      <c r="I5" s="9">
         <v>44649</v>
       </c>
     </row>
     <row r="6" ht="108.6" customHeight="1" spans="1:9">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="6">
         <v>1</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="6">
         <v>1</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="12">
+      <c r="G6" s="6"/>
+      <c r="H6" s="9">
         <v>44640</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="9">
         <v>44640</v>
       </c>
     </row>
-    <row r="7" ht="53" spans="1:9">
-      <c r="A7" s="5" t="s">
+    <row r="7" ht="41.4" spans="1:9">
+      <c r="A7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="6">
         <v>2</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="6">
         <v>1</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="12">
+      <c r="G7" s="6"/>
+      <c r="H7" s="9">
         <v>44643</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="9">
         <v>44646</v>
       </c>
     </row>
-    <row r="8" ht="93" spans="1:9">
-      <c r="A8" s="5" t="s">
+    <row r="8" ht="96.6" spans="1:9">
+      <c r="A8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="6">
         <v>2</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="6">
         <v>1</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="12">
+      <c r="G8" s="6"/>
+      <c r="H8" s="9">
         <v>44642</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="9">
         <v>44644</v>
       </c>
     </row>
-    <row r="9" ht="93" spans="1:9">
-      <c r="A9" s="5" t="s">
+    <row r="9" ht="96.6" spans="1:9">
+      <c r="A9" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="6">
         <v>2</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="6">
         <v>1</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="12">
+      <c r="G9" s="6"/>
+      <c r="H9" s="9">
         <v>44642</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I9" s="9">
         <v>44644</v>
       </c>
     </row>
-    <row r="10" ht="66" spans="1:9">
-      <c r="A10" s="5" t="s">
+    <row r="10" ht="69" spans="1:9">
+      <c r="A10" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="6">
         <v>3</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="6">
         <v>1</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="12">
+      <c r="G10" s="6"/>
+      <c r="H10" s="9">
         <v>44642</v>
       </c>
-      <c r="I10" s="12">
+      <c r="I10" s="9">
         <v>44648</v>
       </c>
     </row>
-    <row r="11" ht="80" spans="1:9">
-      <c r="A11" s="5" t="s">
+    <row r="11" ht="82.8" spans="1:9">
+      <c r="A11" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="6">
         <v>3</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="6">
         <v>1</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="12">
+      <c r="G11" s="6"/>
+      <c r="H11" s="9">
         <v>44639</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="9">
         <v>44641</v>
       </c>
     </row>
-    <row r="12" ht="80" spans="1:9">
-      <c r="A12" s="5" t="s">
+    <row r="12" ht="82.8" spans="1:9">
+      <c r="A12" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="6">
         <v>3</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="6">
         <v>1</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="12">
+      <c r="G12" s="6"/>
+      <c r="H12" s="9">
         <v>44642</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I12" s="9">
         <v>44643</v>
       </c>
     </row>
-    <row r="13" ht="80" spans="1:9">
-      <c r="A13" s="9">
+    <row r="13" ht="82.8" spans="1:9">
+      <c r="A13" s="15">
         <v>1.4</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="6">
         <v>3</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="6">
         <v>1</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="12">
+      <c r="G13" s="6"/>
+      <c r="H13" s="9">
         <v>44645</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I13" s="9">
         <v>44647</v>
       </c>
     </row>
     <row r="14" ht="85.2" customHeight="1" spans="1:9">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="6">
         <v>4</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="6">
         <v>1</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="12">
+      <c r="G14" s="6"/>
+      <c r="H14" s="9">
         <v>44639</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="9">
         <v>44643</v>
       </c>
     </row>
-    <row r="15" ht="66" spans="1:9">
-      <c r="A15" s="9">
+    <row r="15" ht="55.2" spans="1:9">
+      <c r="A15" s="15">
         <v>2.1</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="6">
         <v>2</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="6">
         <v>2</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="12">
+      <c r="G15" s="6"/>
+      <c r="H15" s="9">
         <v>44659</v>
       </c>
-      <c r="I15" s="12">
+      <c r="I15" s="9">
         <v>44662</v>
       </c>
     </row>
-    <row r="16" ht="66" spans="1:9">
-      <c r="A16" s="9">
+    <row r="16" ht="69" spans="1:9">
+      <c r="A16" s="15">
         <v>2.2</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="6">
         <v>1</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="6">
         <v>2</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="12">
+      <c r="G16" s="6"/>
+      <c r="H16" s="9">
         <v>44662</v>
       </c>
-      <c r="I16" s="12">
+      <c r="I16" s="9">
         <v>44662</v>
       </c>
     </row>
-    <row r="17" ht="66" spans="1:9">
-      <c r="A17" s="9">
+    <row r="17" ht="55.2" spans="1:9">
+      <c r="A17" s="15">
         <v>2.3</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="6">
         <v>2</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="6">
         <v>2</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="F17" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="G17" s="5"/>
-      <c r="H17" s="12">
+      <c r="G17" s="6"/>
+      <c r="H17" s="9">
         <v>44661</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="9">
         <v>44661</v>
       </c>
     </row>
-    <row r="18" ht="53" spans="1:9">
-      <c r="A18" s="9">
+    <row r="18" ht="55.2" spans="1:9">
+      <c r="A18" s="15">
         <v>2.4</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="6">
         <v>3</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="6">
         <v>2</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="12">
+      <c r="G18" s="6"/>
+      <c r="H18" s="9">
         <v>44662</v>
       </c>
-      <c r="I18" s="12">
+      <c r="I18" s="9">
         <v>44662</v>
       </c>
     </row>
-    <row r="19" ht="66" spans="1:9">
-      <c r="A19" s="9">
+    <row r="19" ht="69" spans="1:9">
+      <c r="A19" s="15">
         <v>2.5</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="6">
         <v>2</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="6">
         <v>2</v>
       </c>
-      <c r="F19" s="15" t="s">
+      <c r="F19" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="G19" s="5"/>
-      <c r="H19" s="12">
+      <c r="G19" s="6"/>
+      <c r="H19" s="9">
         <v>44662</v>
       </c>
-      <c r="I19" s="12">
+      <c r="I19" s="9">
         <v>44662</v>
       </c>
     </row>
-    <row r="20" ht="66" spans="1:9">
-      <c r="A20" s="9">
+    <row r="20" ht="55.2" spans="1:9">
+      <c r="A20" s="15">
         <v>2.6</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="6">
         <v>3</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="6">
         <v>2</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="F20" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="G20" s="5"/>
-      <c r="H20" s="12">
+      <c r="G20" s="6"/>
+      <c r="H20" s="9">
         <v>44662</v>
       </c>
-      <c r="I20" s="12">
+      <c r="I20" s="9">
         <v>44662</v>
+      </c>
+    </row>
+    <row r="21" ht="60" customHeight="1" spans="1:9">
+      <c r="A21" s="16">
+        <v>2.7</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="17">
+        <v>4</v>
+      </c>
+      <c r="E21" s="17">
+        <v>2</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" s="17"/>
+      <c r="H21" s="9">
+        <v>44664</v>
+      </c>
+      <c r="I21" s="9">
+        <v>44664</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix stories of iteration 4
</commit_message>
<xml_diff>
--- a/Docs/product backlog.xlsx
+++ b/Docs/product backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="13920"/>
+    <workbookView windowHeight="17520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132">
   <si>
     <t>Story ID</t>
   </si>
@@ -416,20 +416,143 @@
   <si>
     <t>- Verify that config includes theme color entry
 - Verify that theme color changes according to config settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should not run if failed to load config
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  As a         airport manager
+  I want      the software not to run if it fails to load any configuration items
+  So that    service with defect will not be provided to users</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-Verify that if any configuration entry is missing or invalid, the programme does not launch
+-Verify that when launch is aborted, admin is informed of problematic entries
+</t>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">heck </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>card numbers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">  As an airline stuff        
+  I want to ensure that the text field can only be accepted 8 digits card number
+  So that card number can be unified</t>
+  </si>
+  <si>
+    <t>-Verify that there will be a warning if the card number is not 8 digits.</t>
+  </si>
+  <si>
+    <t>Configurable auto dark theme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  As an airport staff,
+  I want to decide if the software should change to dark theme when the night falls,
+  So that passengers can have a better check-in experience.</t>
+  </si>
+  <si>
+    <t>- Verify that instance variables change only at the end of a check-in process.
+- Verify that the theme will reset to the previous light theme the next morning.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display aircraft information  </t>
+  </si>
+  <si>
+    <t>As a passenger
+I want to be able to know the aircraft information
+So that I can make sure I'm checking in the right flight</t>
+  </si>
+  <si>
+    <t>- Verify that aircraft information includes plane model, capacity and airline.
+- Verify that the aircraft information window is foldable.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi-platform DB operator   </t>
+  </si>
+  <si>
+    <t>As an airport manager,
+I want to check the correctness of the whole program by using tests,
+and tests should have abilities to run on different OSs.</t>
+  </si>
+  <si>
+    <t>- Verify that tests can run on different OSs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No-operation detection </t>
+  </si>
+  <si>
+    <t>As an airport manager,
+I want the program back to the welcome page if no operation at the login page in a fixed time.</t>
+  </si>
+  <si>
+    <t>- Verify that detection is accurate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Configuration should use less I/O </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  As a         airport manager
+  I want      the software only use I/O once when launching the software
+  So that    performance is optimized</t>
+  </si>
+  <si>
+    <t>-  Verify that I/O operation only happen once when launching software</t>
+  </si>
+  <si>
+    <t>Animations after pressing "Pay"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  As a        passenger
+  I want      there's an animation in the payment screen 
+  So that    make sure I finish paying</t>
+  </si>
+  <si>
+    <t>-  Verify that animation only appears when done</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="0.00_ "/>
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -450,8 +573,28 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -465,43 +608,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -510,9 +616,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -535,16 +640,47 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -563,17 +699,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -588,17 +724,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="33">
@@ -616,43 +751,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -664,133 +871,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -822,6 +957,15 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4"/>
       </bottom>
@@ -833,17 +977,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -864,6 +997,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -878,17 +1026,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -907,162 +1051,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1085,8 +1220,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1109,6 +1244,7 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1457,10 +1593,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="99" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2"/>
@@ -2263,7 +2399,7 @@
       </c>
     </row>
     <row r="30" s="2" customFormat="1" ht="66" spans="1:9">
-      <c r="A30" s="10">
+      <c r="A30" s="7">
         <v>3.1</v>
       </c>
       <c r="B30" s="7" t="s">
@@ -2288,6 +2424,246 @@
       <c r="I30" s="13">
         <v>44673</v>
       </c>
+    </row>
+    <row r="31" ht="80" spans="1:8">
+      <c r="A31" s="7">
+        <v>4.1</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D31" s="5">
+        <v>2</v>
+      </c>
+      <c r="E31" s="5">
+        <v>4</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="G31"/>
+      <c r="H31" s="13"/>
+    </row>
+    <row r="32" ht="53" spans="1:9">
+      <c r="A32" s="7">
+        <v>4.2</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D32" s="5">
+        <v>2</v>
+      </c>
+      <c r="E32" s="5">
+        <v>4</v>
+      </c>
+      <c r="F32" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="G32"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+    </row>
+    <row r="33" ht="80" spans="1:9">
+      <c r="A33" s="7">
+        <v>4.3</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D33" s="5">
+        <v>4</v>
+      </c>
+      <c r="E33" s="5">
+        <v>4</v>
+      </c>
+      <c r="F33" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="G33"/>
+      <c r="H33" s="13">
+        <v>44687</v>
+      </c>
+      <c r="I33" s="13">
+        <v>44688</v>
+      </c>
+    </row>
+    <row r="34" ht="66" spans="1:9">
+      <c r="A34" s="7">
+        <v>4.4</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D34" s="5">
+        <v>3</v>
+      </c>
+      <c r="E34" s="5">
+        <v>4</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="G34"/>
+      <c r="H34" s="13">
+        <v>44687</v>
+      </c>
+      <c r="I34" s="13">
+        <v>44687</v>
+      </c>
+    </row>
+    <row r="35" ht="66" spans="1:9">
+      <c r="A35" s="7">
+        <v>4.5</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D35" s="5">
+        <v>4</v>
+      </c>
+      <c r="E35" s="5">
+        <v>4</v>
+      </c>
+      <c r="F35" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="G35"/>
+      <c r="H35" s="13">
+        <v>44688</v>
+      </c>
+      <c r="I35" s="13">
+        <v>44689</v>
+      </c>
+    </row>
+    <row r="36" ht="53" spans="1:9">
+      <c r="A36" s="7">
+        <v>4.6</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D36" s="5">
+        <v>4</v>
+      </c>
+      <c r="E36" s="5">
+        <v>4</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="G36"/>
+      <c r="H36" s="13">
+        <v>44688</v>
+      </c>
+      <c r="I36" s="13">
+        <v>44689</v>
+      </c>
+    </row>
+    <row r="37" ht="53" spans="1:9">
+      <c r="A37" s="7">
+        <v>4.7</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D37" s="5">
+        <v>4</v>
+      </c>
+      <c r="E37" s="5">
+        <v>4</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="G37"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+    </row>
+    <row r="38" ht="53" spans="1:9">
+      <c r="A38" s="7">
+        <v>4.8</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D38" s="5">
+        <v>4</v>
+      </c>
+      <c r="E38" s="5">
+        <v>4</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="G38"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+    </row>
+    <row r="39" ht="14.8" spans="1:9">
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="I39" s="13"/>
+    </row>
+    <row r="40" spans="9:9">
+      <c r="I40" s="13"/>
+    </row>
+    <row r="41" spans="9:9">
+      <c r="I41" s="13"/>
+    </row>
+    <row r="42" spans="9:9">
+      <c r="I42" s="13"/>
+    </row>
+    <row r="43" spans="9:9">
+      <c r="I43" s="13"/>
+    </row>
+    <row r="44" spans="9:9">
+      <c r="I44" s="13"/>
+    </row>
+    <row r="45" spans="9:9">
+      <c r="I45" s="13"/>
+    </row>
+    <row r="46" spans="9:9">
+      <c r="I46" s="13"/>
+    </row>
+    <row r="47" spans="9:9">
+      <c r="I47" s="13"/>
+    </row>
+    <row r="48" spans="9:9">
+      <c r="I48" s="13"/>
+    </row>
+    <row r="49" spans="9:9">
+      <c r="I49" s="13"/>
     </row>
   </sheetData>
   <sortState ref="A2:I28">

</xml_diff>

<commit_message>
#66 update user story and backlog
</commit_message>
<xml_diff>
--- a/Docs/product backlog.xlsx
+++ b/Docs/product backlog.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\shit\EBU6304-2021-Software-Engineering-Group-111\Docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowHeight="17520"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="17520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="132">
   <si>
     <t>Story ID</t>
   </si>
@@ -440,7 +445,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">heck </t>
     </r>
@@ -458,7 +463,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -545,14 +550,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="25">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -564,53 +563,23 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -620,123 +589,15 @@
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -745,192 +606,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -953,256 +634,17 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1223,7 +665,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1246,61 +688,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
+    <cellStyle name="40% - 着色 1" xfId="1" builtinId="31"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
-    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
-    <cellStyle name="输入" xfId="4" builtinId="20"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
-    <cellStyle name="货币" xfId="7" builtinId="4"/>
-    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
-    <cellStyle name="百分比" xfId="9" builtinId="5"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
-    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
-    <cellStyle name="计算" xfId="15" builtinId="22"/>
-    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
-    <cellStyle name="适中" xfId="17" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
-    <cellStyle name="好" xfId="19" builtinId="26"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="差" xfId="22" builtinId="27"/>
-    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
-    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
-    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
-    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
-    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
-    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
-    <cellStyle name="标题" xfId="33" builtinId="15"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
-    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="注释" xfId="37" builtinId="10"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
-    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
-    <cellStyle name="超链接" xfId="41" builtinId="8"/>
-    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
-    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
-    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1587,33 +986,33 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" zoomScaleNormal="119" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="36" style="2" customWidth="1"/>
     <col min="4" max="4" width="9" style="2"/>
-    <col min="5" max="5" width="21.875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="37.625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="6.125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="24.875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="26.375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="37.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="6.109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="24.88671875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="26.33203125" style="2" customWidth="1"/>
     <col min="10" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1642,7 +1041,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" ht="66" spans="1:9">
+    <row r="2" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
@@ -1669,7 +1068,7 @@
         <v>44644</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" ht="66" spans="1:9">
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="69" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
@@ -1696,7 +1095,7 @@
         <v>44641</v>
       </c>
     </row>
-    <row r="4" ht="93" spans="1:9">
+    <row r="4" spans="1:9" ht="96.6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
@@ -1723,7 +1122,7 @@
         <v>44643</v>
       </c>
     </row>
-    <row r="5" ht="53" spans="1:9">
+    <row r="5" spans="1:9" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -1750,7 +1149,7 @@
         <v>44649</v>
       </c>
     </row>
-    <row r="6" ht="108.6" customHeight="1" spans="1:9">
+    <row r="6" spans="1:9" ht="108.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>25</v>
       </c>
@@ -1777,7 +1176,7 @@
         <v>44640</v>
       </c>
     </row>
-    <row r="7" ht="53" spans="1:9">
+    <row r="7" spans="1:9" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
@@ -1804,7 +1203,7 @@
         <v>44646</v>
       </c>
     </row>
-    <row r="8" ht="93" spans="1:9">
+    <row r="8" spans="1:9" ht="96.6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>33</v>
       </c>
@@ -1831,7 +1230,7 @@
         <v>44644</v>
       </c>
     </row>
-    <row r="9" ht="93" spans="1:9">
+    <row r="9" spans="1:9" ht="96.6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>37</v>
       </c>
@@ -1858,7 +1257,7 @@
         <v>44644</v>
       </c>
     </row>
-    <row r="10" ht="66" spans="1:9">
+    <row r="10" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>40</v>
       </c>
@@ -1885,7 +1284,7 @@
         <v>44648</v>
       </c>
     </row>
-    <row r="11" ht="80" spans="1:9">
+    <row r="11" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>44</v>
       </c>
@@ -1912,7 +1311,7 @@
         <v>44641</v>
       </c>
     </row>
-    <row r="12" ht="80" spans="1:9">
+    <row r="12" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>48</v>
       </c>
@@ -1939,7 +1338,7 @@
         <v>44643</v>
       </c>
     </row>
-    <row r="13" ht="80" spans="1:9">
+    <row r="13" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>1.4</v>
       </c>
@@ -1966,7 +1365,7 @@
         <v>44647</v>
       </c>
     </row>
-    <row r="14" ht="85.15" customHeight="1" spans="1:9">
+    <row r="14" spans="1:9" ht="85.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>55</v>
       </c>
@@ -1993,7 +1392,7 @@
         <v>44643</v>
       </c>
     </row>
-    <row r="15" ht="66" spans="1:9">
+    <row r="15" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>2.1</v>
       </c>
@@ -2020,9 +1419,9 @@
         <v>44662</v>
       </c>
     </row>
-    <row r="16" ht="66" spans="1:9">
+    <row r="16" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>62</v>
@@ -2047,9 +1446,9 @@
         <v>44662</v>
       </c>
     </row>
-    <row r="17" ht="66" spans="1:9">
+    <row r="17" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>65</v>
@@ -2074,7 +1473,7 @@
         <v>44661</v>
       </c>
     </row>
-    <row r="18" ht="53" spans="1:9">
+    <row r="18" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>2.4</v>
       </c>
@@ -2101,7 +1500,7 @@
         <v>44662</v>
       </c>
     </row>
-    <row r="19" ht="66" spans="1:9">
+    <row r="19" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>2.5</v>
       </c>
@@ -2128,7 +1527,7 @@
         <v>44662</v>
       </c>
     </row>
-    <row r="20" ht="66" spans="1:9">
+    <row r="20" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>2.6</v>
       </c>
@@ -2155,7 +1554,7 @@
         <v>44662</v>
       </c>
     </row>
-    <row r="21" s="2" customFormat="1" ht="66" spans="1:9">
+    <row r="21" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>3.1</v>
       </c>
@@ -2182,7 +1581,7 @@
         <v>44672</v>
       </c>
     </row>
-    <row r="22" ht="66" spans="1:9">
+    <row r="22" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>3.2</v>
       </c>
@@ -2209,7 +1608,7 @@
         <v>44667</v>
       </c>
     </row>
-    <row r="23" ht="66" spans="1:9">
+    <row r="23" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>3.3</v>
       </c>
@@ -2236,7 +1635,7 @@
         <v>44670</v>
       </c>
     </row>
-    <row r="24" s="2" customFormat="1" ht="53" spans="1:9">
+    <row r="24" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>3.4</v>
       </c>
@@ -2263,7 +1662,7 @@
         <v>44677</v>
       </c>
     </row>
-    <row r="25" s="2" customFormat="1" ht="66" spans="1:9">
+    <row r="25" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>3.5</v>
       </c>
@@ -2290,7 +1689,7 @@
         <v>44670</v>
       </c>
     </row>
-    <row r="26" s="2" customFormat="1" ht="66" spans="1:9">
+    <row r="26" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>3.6</v>
       </c>
@@ -2317,7 +1716,7 @@
         <v>44671</v>
       </c>
     </row>
-    <row r="27" s="2" customFormat="1" ht="66" customHeight="1" spans="1:9">
+    <row r="27" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>3.7</v>
       </c>
@@ -2344,7 +1743,7 @@
         <v>44674</v>
       </c>
     </row>
-    <row r="28" s="2" customFormat="1" ht="80" spans="1:9">
+    <row r="28" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>3.8</v>
       </c>
@@ -2371,7 +1770,7 @@
         <v>44675</v>
       </c>
     </row>
-    <row r="29" ht="53" spans="1:9">
+    <row r="29" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>3.9</v>
       </c>
@@ -2398,7 +1797,7 @@
         <v>44677</v>
       </c>
     </row>
-    <row r="30" s="2" customFormat="1" ht="66" spans="1:9">
+    <row r="30" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>3.1</v>
       </c>
@@ -2425,9 +1824,9 @@
         <v>44673</v>
       </c>
     </row>
-    <row r="31" ht="80" spans="1:8">
+    <row r="31" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>107</v>
@@ -2447,7 +1846,7 @@
       <c r="G31"/>
       <c r="H31" s="13"/>
     </row>
-    <row r="32" ht="53" spans="1:9">
+    <row r="32" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>4.2</v>
       </c>
@@ -2470,7 +1869,7 @@
       <c r="H32" s="13"/>
       <c r="I32" s="13"/>
     </row>
-    <row r="33" ht="80" spans="1:9">
+    <row r="33" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>4.3</v>
       </c>
@@ -2497,9 +1896,9 @@
         <v>44688</v>
       </c>
     </row>
-    <row r="34" ht="66" spans="1:9">
+    <row r="34" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>116</v>
@@ -2521,10 +1920,10 @@
         <v>44687</v>
       </c>
       <c r="I34" s="13">
-        <v>44687</v>
-      </c>
-    </row>
-    <row r="35" ht="66" spans="1:9">
+        <v>44692</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>4.5</v>
       </c>
@@ -2551,9 +1950,9 @@
         <v>44689</v>
       </c>
     </row>
-    <row r="36" ht="53" spans="1:9">
+    <row r="36" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>122</v>
@@ -2578,7 +1977,7 @@
         <v>44689</v>
       </c>
     </row>
-    <row r="37" ht="53" spans="1:9">
+    <row r="37" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>4.7</v>
       </c>
@@ -2601,7 +2000,7 @@
       <c r="H37" s="13"/>
       <c r="I37" s="13"/>
     </row>
-    <row r="38" ht="53" spans="1:9">
+    <row r="38" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>4.8</v>
       </c>
@@ -2624,7 +2023,7 @@
       <c r="H38" s="13"/>
       <c r="I38" s="13"/>
     </row>
-    <row r="39" ht="14.8" spans="1:9">
+    <row r="39" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="10"/>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
@@ -2635,42 +2034,42 @@
       </c>
       <c r="I39" s="13"/>
     </row>
-    <row r="40" spans="9:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I40" s="13"/>
     </row>
-    <row r="41" spans="9:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I41" s="13"/>
     </row>
-    <row r="42" spans="9:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I42" s="13"/>
     </row>
-    <row r="43" spans="9:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I43" s="13"/>
     </row>
-    <row r="44" spans="9:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I44" s="13"/>
     </row>
-    <row r="45" spans="9:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I45" s="13"/>
     </row>
-    <row r="46" spans="9:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I46" s="13"/>
     </row>
-    <row r="47" spans="9:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I47" s="13"/>
     </row>
-    <row r="48" spans="9:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I48" s="13"/>
     </row>
-    <row r="49" spans="9:9">
+    <row r="49" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I49" s="13"/>
     </row>
   </sheetData>
   <sortState ref="A2:I28">
     <sortCondition ref="D2"/>
   </sortState>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Amend story 4.8 and backlog.
</commit_message>
<xml_diff>
--- a/Docs/product backlog.xlsx
+++ b/Docs/product backlog.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EBU6304-2021-Software-Engineering-Group-111\Docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510F3E4C-6DB6-462E-8A62-FC830FCACF99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="17520"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="132">
   <si>
     <t>Story ID</t>
   </si>
@@ -440,7 +446,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">heck </t>
     </r>
@@ -458,7 +464,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <charset val="134"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -545,15 +551,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -565,70 +567,25 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
-      <charset val="134"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -636,114 +593,16 @@
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="9"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -752,192 +611,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -960,256 +639,17 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="47" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1236,7 +676,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1262,61 +702,18 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
+    <cellStyle name="40% - 着色 1" xfId="1" builtinId="31"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
-    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
-    <cellStyle name="输入" xfId="4" builtinId="20"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
-    <cellStyle name="货币" xfId="7" builtinId="4"/>
-    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
-    <cellStyle name="百分比" xfId="9" builtinId="5"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
-    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
-    <cellStyle name="计算" xfId="15" builtinId="22"/>
-    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
-    <cellStyle name="适中" xfId="17" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
-    <cellStyle name="好" xfId="19" builtinId="26"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
-    <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="差" xfId="22" builtinId="27"/>
-    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
-    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
-    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
-    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
-    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
-    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
-    <cellStyle name="标题" xfId="33" builtinId="15"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
-    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="注释" xfId="37" builtinId="10"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
-    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
-    <cellStyle name="超链接" xfId="41" builtinId="8"/>
-    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
-    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
-    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1603,33 +1000,33 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.8846153846154" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.3365384615385" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="36" style="2" customWidth="1"/>
     <col min="4" max="4" width="9" style="2"/>
-    <col min="5" max="5" width="21.8846153846154" style="2" customWidth="1"/>
-    <col min="6" max="6" width="37.6634615384615" style="3" customWidth="1"/>
-    <col min="7" max="7" width="6.10576923076923" style="2" customWidth="1"/>
-    <col min="8" max="8" width="24.8846153846154" style="2" customWidth="1"/>
-    <col min="9" max="9" width="26.3365384615385" style="2" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="37.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="6.109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="24.88671875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="26.33203125" style="2" customWidth="1"/>
     <col min="10" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1658,7 +1055,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" ht="66" spans="1:9">
+    <row r="2" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
@@ -1685,7 +1082,7 @@
         <v>44644</v>
       </c>
     </row>
-    <row r="3" s="1" customFormat="1" ht="66" spans="1:9">
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="69" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
@@ -1712,7 +1109,7 @@
         <v>44641</v>
       </c>
     </row>
-    <row r="4" ht="93" spans="1:9">
+    <row r="4" spans="1:9" ht="96.6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>17</v>
       </c>
@@ -1739,7 +1136,7 @@
         <v>44643</v>
       </c>
     </row>
-    <row r="5" ht="53" spans="1:9">
+    <row r="5" spans="1:9" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
@@ -1766,7 +1163,7 @@
         <v>44649</v>
       </c>
     </row>
-    <row r="6" ht="108.6" customHeight="1" spans="1:9">
+    <row r="6" spans="1:9" ht="108.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>25</v>
       </c>
@@ -1793,7 +1190,7 @@
         <v>44640</v>
       </c>
     </row>
-    <row r="7" ht="53" spans="1:9">
+    <row r="7" spans="1:9" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
@@ -1820,7 +1217,7 @@
         <v>44646</v>
       </c>
     </row>
-    <row r="8" ht="93" spans="1:9">
+    <row r="8" spans="1:9" ht="96.6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>33</v>
       </c>
@@ -1847,7 +1244,7 @@
         <v>44644</v>
       </c>
     </row>
-    <row r="9" ht="93" spans="1:9">
+    <row r="9" spans="1:9" ht="96.6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>37</v>
       </c>
@@ -1874,7 +1271,7 @@
         <v>44644</v>
       </c>
     </row>
-    <row r="10" ht="66" spans="1:9">
+    <row r="10" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>40</v>
       </c>
@@ -1901,7 +1298,7 @@
         <v>44648</v>
       </c>
     </row>
-    <row r="11" ht="80" spans="1:9">
+    <row r="11" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>44</v>
       </c>
@@ -1928,7 +1325,7 @@
         <v>44641</v>
       </c>
     </row>
-    <row r="12" ht="80" spans="1:9">
+    <row r="12" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>48</v>
       </c>
@@ -1955,7 +1352,7 @@
         <v>44643</v>
       </c>
     </row>
-    <row r="13" ht="80" spans="1:9">
+    <row r="13" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>1.4</v>
       </c>
@@ -1982,7 +1379,7 @@
         <v>44647</v>
       </c>
     </row>
-    <row r="14" ht="85.2" customHeight="1" spans="1:9">
+    <row r="14" spans="1:9" ht="85.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>55</v>
       </c>
@@ -2009,7 +1406,7 @@
         <v>44643</v>
       </c>
     </row>
-    <row r="15" ht="66" spans="1:9">
+    <row r="15" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>2.1</v>
       </c>
@@ -2036,9 +1433,9 @@
         <v>44662</v>
       </c>
     </row>
-    <row r="16" ht="66" spans="1:9">
+    <row r="16" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>62</v>
@@ -2063,9 +1460,9 @@
         <v>44662</v>
       </c>
     </row>
-    <row r="17" ht="66" spans="1:9">
+    <row r="17" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>65</v>
@@ -2090,7 +1487,7 @@
         <v>44661</v>
       </c>
     </row>
-    <row r="18" ht="53" spans="1:9">
+    <row r="18" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>2.4</v>
       </c>
@@ -2117,7 +1514,7 @@
         <v>44662</v>
       </c>
     </row>
-    <row r="19" ht="66" spans="1:9">
+    <row r="19" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>2.5</v>
       </c>
@@ -2144,7 +1541,7 @@
         <v>44662</v>
       </c>
     </row>
-    <row r="20" ht="66" spans="1:9">
+    <row r="20" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>2.6</v>
       </c>
@@ -2171,7 +1568,7 @@
         <v>44662</v>
       </c>
     </row>
-    <row r="21" ht="66" spans="1:9">
+    <row r="21" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>3.1</v>
       </c>
@@ -2198,7 +1595,7 @@
         <v>44672</v>
       </c>
     </row>
-    <row r="22" ht="66" spans="1:9">
+    <row r="22" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>3.2</v>
       </c>
@@ -2225,7 +1622,7 @@
         <v>44667</v>
       </c>
     </row>
-    <row r="23" ht="66" spans="1:9">
+    <row r="23" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>3.3</v>
       </c>
@@ -2252,7 +1649,7 @@
         <v>44670</v>
       </c>
     </row>
-    <row r="24" ht="53" spans="1:9">
+    <row r="24" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>3.4</v>
       </c>
@@ -2279,7 +1676,7 @@
         <v>44677</v>
       </c>
     </row>
-    <row r="25" ht="66" spans="1:9">
+    <row r="25" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>3.5</v>
       </c>
@@ -2306,7 +1703,7 @@
         <v>44670</v>
       </c>
     </row>
-    <row r="26" ht="66" spans="1:9">
+    <row r="26" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>3.6</v>
       </c>
@@ -2333,7 +1730,7 @@
         <v>44671</v>
       </c>
     </row>
-    <row r="27" ht="66" customHeight="1" spans="1:9">
+    <row r="27" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>3.7</v>
       </c>
@@ -2360,7 +1757,7 @@
         <v>44674</v>
       </c>
     </row>
-    <row r="28" ht="80" spans="1:9">
+    <row r="28" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>3.8</v>
       </c>
@@ -2387,7 +1784,7 @@
         <v>44675</v>
       </c>
     </row>
-    <row r="29" ht="53" spans="1:9">
+    <row r="29" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>3.9</v>
       </c>
@@ -2414,7 +1811,7 @@
         <v>44677</v>
       </c>
     </row>
-    <row r="30" ht="66" spans="1:9">
+    <row r="30" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>3.1</v>
       </c>
@@ -2441,9 +1838,9 @@
         <v>44673</v>
       </c>
     </row>
-    <row r="31" ht="80" spans="1:9">
+    <row r="31" spans="1:9" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="B31" s="10" t="s">
         <v>107</v>
@@ -2468,7 +1865,7 @@
         <v>44691</v>
       </c>
     </row>
-    <row r="32" ht="53" spans="1:9">
+    <row r="32" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>4.2</v>
       </c>
@@ -2495,7 +1892,7 @@
         <v>44692</v>
       </c>
     </row>
-    <row r="33" s="2" customFormat="1" ht="66" spans="1:9">
+    <row r="33" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>4.3</v>
       </c>
@@ -2522,9 +1919,9 @@
         <v>44692</v>
       </c>
     </row>
-    <row r="34" ht="80" spans="1:9">
+    <row r="34" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="B34" s="10" t="s">
         <v>116</v>
@@ -2549,7 +1946,7 @@
         <v>44688</v>
       </c>
     </row>
-    <row r="35" ht="66" spans="1:9">
+    <row r="35" spans="1:9" ht="69" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>4.5</v>
       </c>
@@ -2576,9 +1973,9 @@
         <v>44689</v>
       </c>
     </row>
-    <row r="36" ht="53" spans="1:9">
+    <row r="36" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>122</v>
@@ -2603,7 +2000,7 @@
         <v>44689</v>
       </c>
     </row>
-    <row r="37" ht="53" spans="1:9">
+    <row r="37" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>4.7</v>
       </c>
@@ -2630,7 +2027,7 @@
         <v>44687</v>
       </c>
     </row>
-    <row r="38" ht="53" spans="1:9">
+    <row r="38" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>4.8</v>
       </c>
@@ -2651,13 +2048,13 @@
       </c>
       <c r="G38"/>
       <c r="H38" s="15">
-        <v>44687</v>
+        <v>44691</v>
       </c>
       <c r="I38" s="15">
-        <v>44688</v>
-      </c>
-    </row>
-    <row r="39" ht="14.8" spans="1:9">
+        <v>44693</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="12"/>
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
@@ -2668,42 +2065,42 @@
       </c>
       <c r="I39" s="15"/>
     </row>
-    <row r="40" spans="9:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I40" s="15"/>
     </row>
-    <row r="41" spans="9:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I41" s="15"/>
     </row>
-    <row r="42" spans="9:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I42" s="15"/>
     </row>
-    <row r="43" spans="9:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I43" s="15"/>
     </row>
-    <row r="44" spans="9:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I44" s="15"/>
     </row>
-    <row r="45" spans="9:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I45" s="15"/>
     </row>
-    <row r="46" spans="9:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I46" s="15"/>
     </row>
-    <row r="47" spans="9:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I47" s="15"/>
     </row>
-    <row r="48" spans="9:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I48" s="15"/>
     </row>
-    <row r="49" spans="9:9">
+    <row r="49" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I49" s="15"/>
     </row>
   </sheetData>
-  <sortState ref="A2:I28">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I28">
     <sortCondition ref="D2"/>
   </sortState>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>